<commit_message>
update scraping.py to include Registration No mapping and save to new Excel file; modify .gitignore to exclude additional files
</commit_message>
<xml_diff>
--- a/college_data.xlsx
+++ b/college_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H174"/>
+  <dimension ref="A1:I174"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,6 +462,11 @@
           <t>Status</t>
         </is>
       </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Registration No</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -502,6 +507,7 @@
       <c r="H2" t="n">
         <v>1</v>
       </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -542,6 +548,7 @@
       <c r="H3" t="n">
         <v>1</v>
       </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -582,6 +589,7 @@
       <c r="H4" t="n">
         <v>1</v>
       </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -622,6 +630,7 @@
       <c r="H5" t="n">
         <v>1</v>
       </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -662,6 +671,7 @@
       <c r="H6" t="n">
         <v>1</v>
       </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -702,6 +712,7 @@
       <c r="H7" t="n">
         <v>1</v>
       </c>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -742,6 +753,7 @@
       <c r="H8" t="n">
         <v>1</v>
       </c>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -782,6 +794,7 @@
       <c r="H9" t="n">
         <v>1</v>
       </c>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -822,6 +835,7 @@
       <c r="H10" t="n">
         <v>1</v>
       </c>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -862,6 +876,7 @@
       <c r="H11" t="n">
         <v>1</v>
       </c>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -902,6 +917,7 @@
       <c r="H12" t="n">
         <v>1</v>
       </c>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -942,6 +958,7 @@
       <c r="H13" t="n">
         <v>1</v>
       </c>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -982,6 +999,7 @@
       <c r="H14" t="n">
         <v>1</v>
       </c>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1022,6 +1040,7 @@
       <c r="H15" t="n">
         <v>1</v>
       </c>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1062,6 +1081,7 @@
       <c r="H16" t="n">
         <v>1</v>
       </c>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1102,6 +1122,7 @@
       <c r="H17" t="n">
         <v>1</v>
       </c>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1142,6 +1163,7 @@
       <c r="H18" t="n">
         <v>1</v>
       </c>
+      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1182,6 +1204,7 @@
       <c r="H19" t="n">
         <v>1</v>
       </c>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1222,6 +1245,7 @@
       <c r="H20" t="n">
         <v>1</v>
       </c>
+      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1262,6 +1286,7 @@
       <c r="H21" t="n">
         <v>1</v>
       </c>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1302,6 +1327,7 @@
       <c r="H22" t="n">
         <v>1</v>
       </c>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1342,6 +1368,7 @@
       <c r="H23" t="n">
         <v>1</v>
       </c>
+      <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1382,6 +1409,7 @@
       <c r="H24" t="n">
         <v>1</v>
       </c>
+      <c r="I24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1422,6 +1450,7 @@
       <c r="H25" t="n">
         <v>1</v>
       </c>
+      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1462,6 +1491,7 @@
       <c r="H26" t="n">
         <v>1</v>
       </c>
+      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1502,6 +1532,7 @@
       <c r="H27" t="n">
         <v>1</v>
       </c>
+      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1542,6 +1573,7 @@
       <c r="H28" t="n">
         <v>1</v>
       </c>
+      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1582,6 +1614,7 @@
       <c r="H29" t="n">
         <v>1</v>
       </c>
+      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1622,6 +1655,7 @@
       <c r="H30" t="n">
         <v>1</v>
       </c>
+      <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1662,6 +1696,7 @@
       <c r="H31" t="n">
         <v>1</v>
       </c>
+      <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1702,6 +1737,7 @@
       <c r="H32" t="n">
         <v>1</v>
       </c>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1742,6 +1778,7 @@
       <c r="H33" t="n">
         <v>1</v>
       </c>
+      <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1782,6 +1819,7 @@
       <c r="H34" t="n">
         <v>1</v>
       </c>
+      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1822,6 +1860,7 @@
       <c r="H35" t="n">
         <v>1</v>
       </c>
+      <c r="I35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1862,6 +1901,7 @@
       <c r="H36" t="n">
         <v>1</v>
       </c>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1902,6 +1942,7 @@
       <c r="H37" t="n">
         <v>1</v>
       </c>
+      <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1942,6 +1983,7 @@
       <c r="H38" t="n">
         <v>1</v>
       </c>
+      <c r="I38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1982,6 +2024,7 @@
       <c r="H39" t="n">
         <v>1</v>
       </c>
+      <c r="I39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2022,6 +2065,7 @@
       <c r="H40" t="n">
         <v>1</v>
       </c>
+      <c r="I40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2062,6 +2106,7 @@
       <c r="H41" t="n">
         <v>1</v>
       </c>
+      <c r="I41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2102,6 +2147,7 @@
       <c r="H42" t="n">
         <v>1</v>
       </c>
+      <c r="I42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2142,6 +2188,7 @@
       <c r="H43" t="n">
         <v>1</v>
       </c>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2182,6 +2229,7 @@
       <c r="H44" t="n">
         <v>1</v>
       </c>
+      <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2222,6 +2270,7 @@
       <c r="H45" t="n">
         <v>1</v>
       </c>
+      <c r="I45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2262,6 +2311,7 @@
       <c r="H46" t="n">
         <v>1</v>
       </c>
+      <c r="I46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2302,6 +2352,7 @@
       <c r="H47" t="n">
         <v>1</v>
       </c>
+      <c r="I47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2342,6 +2393,7 @@
       <c r="H48" t="n">
         <v>1</v>
       </c>
+      <c r="I48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2382,6 +2434,7 @@
       <c r="H49" t="n">
         <v>1</v>
       </c>
+      <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2422,6 +2475,7 @@
       <c r="H50" t="n">
         <v>1</v>
       </c>
+      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2462,6 +2516,7 @@
       <c r="H51" t="n">
         <v>1</v>
       </c>
+      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2502,6 +2557,7 @@
       <c r="H52" t="n">
         <v>1</v>
       </c>
+      <c r="I52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2542,6 +2598,7 @@
       <c r="H53" t="n">
         <v>1</v>
       </c>
+      <c r="I53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2582,6 +2639,7 @@
       <c r="H54" t="n">
         <v>1</v>
       </c>
+      <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2622,6 +2680,7 @@
       <c r="H55" t="n">
         <v>1</v>
       </c>
+      <c r="I55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2662,6 +2721,7 @@
       <c r="H56" t="n">
         <v>1</v>
       </c>
+      <c r="I56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2702,6 +2762,7 @@
       <c r="H57" t="n">
         <v>1</v>
       </c>
+      <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2742,6 +2803,7 @@
       <c r="H58" t="n">
         <v>1</v>
       </c>
+      <c r="I58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2782,6 +2844,7 @@
       <c r="H59" t="n">
         <v>1</v>
       </c>
+      <c r="I59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2822,6 +2885,7 @@
       <c r="H60" t="n">
         <v>1</v>
       </c>
+      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2862,6 +2926,7 @@
       <c r="H61" t="n">
         <v>1</v>
       </c>
+      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2902,6 +2967,7 @@
       <c r="H62" t="n">
         <v>1</v>
       </c>
+      <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2942,6 +3008,7 @@
       <c r="H63" t="n">
         <v>1</v>
       </c>
+      <c r="I63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2982,6 +3049,7 @@
       <c r="H64" t="n">
         <v>1</v>
       </c>
+      <c r="I64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3022,6 +3090,7 @@
       <c r="H65" t="n">
         <v>1</v>
       </c>
+      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3062,6 +3131,7 @@
       <c r="H66" t="n">
         <v>1</v>
       </c>
+      <c r="I66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3102,6 +3172,7 @@
       <c r="H67" t="n">
         <v>1</v>
       </c>
+      <c r="I67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3142,6 +3213,7 @@
       <c r="H68" t="n">
         <v>1</v>
       </c>
+      <c r="I68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3182,6 +3254,7 @@
       <c r="H69" t="n">
         <v>1</v>
       </c>
+      <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3222,6 +3295,7 @@
       <c r="H70" t="n">
         <v>1</v>
       </c>
+      <c r="I70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3262,6 +3336,7 @@
       <c r="H71" t="n">
         <v>1</v>
       </c>
+      <c r="I71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3302,6 +3377,7 @@
       <c r="H72" t="n">
         <v>1</v>
       </c>
+      <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3342,6 +3418,7 @@
       <c r="H73" t="n">
         <v>1</v>
       </c>
+      <c r="I73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3382,6 +3459,7 @@
       <c r="H74" t="n">
         <v>1</v>
       </c>
+      <c r="I74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3422,6 +3500,7 @@
       <c r="H75" t="n">
         <v>1</v>
       </c>
+      <c r="I75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3462,6 +3541,7 @@
       <c r="H76" t="n">
         <v>1</v>
       </c>
+      <c r="I76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3502,6 +3582,7 @@
       <c r="H77" t="n">
         <v>1</v>
       </c>
+      <c r="I77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3542,6 +3623,7 @@
       <c r="H78" t="n">
         <v>1</v>
       </c>
+      <c r="I78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3582,6 +3664,7 @@
       <c r="H79" t="n">
         <v>1</v>
       </c>
+      <c r="I79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3622,6 +3705,7 @@
       <c r="H80" t="n">
         <v>1</v>
       </c>
+      <c r="I80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3662,6 +3746,7 @@
       <c r="H81" t="n">
         <v>1</v>
       </c>
+      <c r="I81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3702,6 +3787,7 @@
       <c r="H82" t="n">
         <v>1</v>
       </c>
+      <c r="I82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3742,6 +3828,7 @@
       <c r="H83" t="n">
         <v>1</v>
       </c>
+      <c r="I83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3782,6 +3869,7 @@
       <c r="H84" t="n">
         <v>1</v>
       </c>
+      <c r="I84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3822,6 +3910,7 @@
       <c r="H85" t="n">
         <v>1</v>
       </c>
+      <c r="I85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3862,6 +3951,7 @@
       <c r="H86" t="n">
         <v>1</v>
       </c>
+      <c r="I86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3902,6 +3992,7 @@
       <c r="H87" t="n">
         <v>1</v>
       </c>
+      <c r="I87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3942,6 +4033,7 @@
       <c r="H88" t="n">
         <v>1</v>
       </c>
+      <c r="I88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3982,6 +4074,7 @@
       <c r="H89" t="n">
         <v>1</v>
       </c>
+      <c r="I89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4022,6 +4115,7 @@
       <c r="H90" t="n">
         <v>1</v>
       </c>
+      <c r="I90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4062,6 +4156,7 @@
       <c r="H91" t="n">
         <v>1</v>
       </c>
+      <c r="I91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4102,6 +4197,7 @@
       <c r="H92" t="n">
         <v>1</v>
       </c>
+      <c r="I92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4142,6 +4238,7 @@
       <c r="H93" t="n">
         <v>1</v>
       </c>
+      <c r="I93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4182,6 +4279,7 @@
       <c r="H94" t="n">
         <v>1</v>
       </c>
+      <c r="I94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4222,6 +4320,7 @@
       <c r="H95" t="n">
         <v>1</v>
       </c>
+      <c r="I95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4262,6 +4361,7 @@
       <c r="H96" t="n">
         <v>1</v>
       </c>
+      <c r="I96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4302,6 +4402,7 @@
       <c r="H97" t="n">
         <v>1</v>
       </c>
+      <c r="I97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4342,6 +4443,7 @@
       <c r="H98" t="n">
         <v>1</v>
       </c>
+      <c r="I98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4382,6 +4484,7 @@
       <c r="H99" t="n">
         <v>1</v>
       </c>
+      <c r="I99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4422,6 +4525,7 @@
       <c r="H100" t="n">
         <v>1</v>
       </c>
+      <c r="I100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4462,6 +4566,7 @@
       <c r="H101" t="n">
         <v>1</v>
       </c>
+      <c r="I101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4502,6 +4607,7 @@
       <c r="H102" t="n">
         <v>1</v>
       </c>
+      <c r="I102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4542,6 +4648,7 @@
       <c r="H103" t="n">
         <v>1</v>
       </c>
+      <c r="I103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4582,6 +4689,7 @@
       <c r="H104" t="n">
         <v>1</v>
       </c>
+      <c r="I104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4622,6 +4730,7 @@
       <c r="H105" t="n">
         <v>1</v>
       </c>
+      <c r="I105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4662,6 +4771,7 @@
       <c r="H106" t="n">
         <v>1</v>
       </c>
+      <c r="I106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4702,6 +4812,7 @@
       <c r="H107" t="n">
         <v>1</v>
       </c>
+      <c r="I107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4742,6 +4853,7 @@
       <c r="H108" t="n">
         <v>1</v>
       </c>
+      <c r="I108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4782,6 +4894,7 @@
       <c r="H109" t="n">
         <v>1</v>
       </c>
+      <c r="I109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4822,6 +4935,7 @@
       <c r="H110" t="n">
         <v>1</v>
       </c>
+      <c r="I110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4862,6 +4976,7 @@
       <c r="H111" t="n">
         <v>1</v>
       </c>
+      <c r="I111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4902,6 +5017,7 @@
       <c r="H112" t="n">
         <v>1</v>
       </c>
+      <c r="I112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4942,6 +5058,7 @@
       <c r="H113" t="n">
         <v>1</v>
       </c>
+      <c r="I113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4982,6 +5099,7 @@
       <c r="H114" t="n">
         <v>1</v>
       </c>
+      <c r="I114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -5022,6 +5140,7 @@
       <c r="H115" t="n">
         <v>1</v>
       </c>
+      <c r="I115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -5062,6 +5181,7 @@
       <c r="H116" t="n">
         <v>1</v>
       </c>
+      <c r="I116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -5102,6 +5222,7 @@
       <c r="H117" t="n">
         <v>1</v>
       </c>
+      <c r="I117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5142,6 +5263,7 @@
       <c r="H118" t="n">
         <v>1</v>
       </c>
+      <c r="I118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -5182,6 +5304,7 @@
       <c r="H119" t="n">
         <v>1</v>
       </c>
+      <c r="I119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -5222,6 +5345,7 @@
       <c r="H120" t="n">
         <v>1</v>
       </c>
+      <c r="I120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -5262,6 +5386,7 @@
       <c r="H121" t="n">
         <v>1</v>
       </c>
+      <c r="I121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5302,6 +5427,7 @@
       <c r="H122" t="n">
         <v>1</v>
       </c>
+      <c r="I122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -5342,6 +5468,7 @@
       <c r="H123" t="n">
         <v>1</v>
       </c>
+      <c r="I123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5382,6 +5509,7 @@
       <c r="H124" t="n">
         <v>1</v>
       </c>
+      <c r="I124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5422,6 +5550,7 @@
       <c r="H125" t="n">
         <v>1</v>
       </c>
+      <c r="I125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5462,6 +5591,7 @@
       <c r="H126" t="n">
         <v>1</v>
       </c>
+      <c r="I126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5502,6 +5632,7 @@
       <c r="H127" t="n">
         <v>1</v>
       </c>
+      <c r="I127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -5542,6 +5673,7 @@
       <c r="H128" t="n">
         <v>1</v>
       </c>
+      <c r="I128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -5582,6 +5714,7 @@
       <c r="H129" t="n">
         <v>1</v>
       </c>
+      <c r="I129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -5622,6 +5755,7 @@
       <c r="H130" t="n">
         <v>1</v>
       </c>
+      <c r="I130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -5662,6 +5796,7 @@
       <c r="H131" t="n">
         <v>1</v>
       </c>
+      <c r="I131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -5702,6 +5837,7 @@
       <c r="H132" t="n">
         <v>1</v>
       </c>
+      <c r="I132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -5742,6 +5878,7 @@
       <c r="H133" t="n">
         <v>1</v>
       </c>
+      <c r="I133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -5782,6 +5919,7 @@
       <c r="H134" t="n">
         <v>1</v>
       </c>
+      <c r="I134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5822,6 +5960,7 @@
       <c r="H135" t="n">
         <v>1</v>
       </c>
+      <c r="I135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -5862,6 +6001,7 @@
       <c r="H136" t="n">
         <v>1</v>
       </c>
+      <c r="I136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -5902,6 +6042,7 @@
       <c r="H137" t="n">
         <v>1</v>
       </c>
+      <c r="I137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5942,6 +6083,7 @@
       <c r="H138" t="n">
         <v>1</v>
       </c>
+      <c r="I138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -5982,6 +6124,7 @@
       <c r="H139" t="n">
         <v>1</v>
       </c>
+      <c r="I139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -6022,6 +6165,7 @@
       <c r="H140" t="n">
         <v>1</v>
       </c>
+      <c r="I140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -6062,6 +6206,7 @@
       <c r="H141" t="n">
         <v>1</v>
       </c>
+      <c r="I141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -6102,6 +6247,7 @@
       <c r="H142" t="n">
         <v>1</v>
       </c>
+      <c r="I142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -6142,6 +6288,7 @@
       <c r="H143" t="n">
         <v>1</v>
       </c>
+      <c r="I143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -6182,6 +6329,7 @@
       <c r="H144" t="n">
         <v>1</v>
       </c>
+      <c r="I144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -6222,6 +6370,7 @@
       <c r="H145" t="n">
         <v>1</v>
       </c>
+      <c r="I145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -6262,6 +6411,7 @@
       <c r="H146" t="n">
         <v>1</v>
       </c>
+      <c r="I146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -6302,6 +6452,7 @@
       <c r="H147" t="n">
         <v>1</v>
       </c>
+      <c r="I147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -6342,6 +6493,7 @@
       <c r="H148" t="n">
         <v>1</v>
       </c>
+      <c r="I148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -6382,6 +6534,7 @@
       <c r="H149" t="n">
         <v>1</v>
       </c>
+      <c r="I149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -6422,6 +6575,7 @@
       <c r="H150" t="n">
         <v>1</v>
       </c>
+      <c r="I150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -6462,6 +6616,7 @@
       <c r="H151" t="n">
         <v>1</v>
       </c>
+      <c r="I151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -6502,6 +6657,7 @@
       <c r="H152" t="n">
         <v>1</v>
       </c>
+      <c r="I152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -6542,6 +6698,7 @@
       <c r="H153" t="n">
         <v>1</v>
       </c>
+      <c r="I153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -6582,6 +6739,7 @@
       <c r="H154" t="n">
         <v>1</v>
       </c>
+      <c r="I154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -6622,6 +6780,7 @@
       <c r="H155" t="n">
         <v>1</v>
       </c>
+      <c r="I155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -6662,6 +6821,7 @@
       <c r="H156" t="n">
         <v>1</v>
       </c>
+      <c r="I156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -6702,6 +6862,7 @@
       <c r="H157" t="n">
         <v>1</v>
       </c>
+      <c r="I157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -6742,6 +6903,7 @@
       <c r="H158" t="n">
         <v>1</v>
       </c>
+      <c r="I158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -6782,6 +6944,7 @@
       <c r="H159" t="n">
         <v>1</v>
       </c>
+      <c r="I159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -6822,6 +6985,7 @@
       <c r="H160" t="n">
         <v>1</v>
       </c>
+      <c r="I160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -6862,6 +7026,7 @@
       <c r="H161" t="n">
         <v>1</v>
       </c>
+      <c r="I161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -6902,6 +7067,7 @@
       <c r="H162" t="n">
         <v>1</v>
       </c>
+      <c r="I162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -6942,6 +7108,7 @@
       <c r="H163" t="n">
         <v>1</v>
       </c>
+      <c r="I163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -6982,6 +7149,7 @@
       <c r="H164" t="n">
         <v>1</v>
       </c>
+      <c r="I164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -7022,6 +7190,7 @@
       <c r="H165" t="n">
         <v>1</v>
       </c>
+      <c r="I165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -7062,6 +7231,7 @@
       <c r="H166" t="n">
         <v>1</v>
       </c>
+      <c r="I166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -7102,6 +7272,7 @@
       <c r="H167" t="n">
         <v>1</v>
       </c>
+      <c r="I167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -7142,6 +7313,7 @@
       <c r="H168" t="n">
         <v>1</v>
       </c>
+      <c r="I168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -7182,6 +7354,7 @@
       <c r="H169" t="n">
         <v>1</v>
       </c>
+      <c r="I169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -7222,6 +7395,7 @@
       <c r="H170" t="n">
         <v>1</v>
       </c>
+      <c r="I170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -7262,6 +7436,7 @@
       <c r="H171" t="n">
         <v>1</v>
       </c>
+      <c r="I171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -7302,6 +7477,7 @@
       <c r="H172" t="n">
         <v>1</v>
       </c>
+      <c r="I172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -7342,6 +7518,7 @@
       <c r="H173" t="n">
         <v>1</v>
       </c>
+      <c r="I173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -7382,6 +7559,7 @@
       <c r="H174" t="n">
         <v>1</v>
       </c>
+      <c r="I174" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>